<commit_message>
Histogram for Each Set
</commit_message>
<xml_diff>
--- a/Assignment_2/temizlenmiş_veri.xlsx
+++ b/Assignment_2/temizlenmiş_veri.xlsx
@@ -2282,7 +2282,7 @@
         <v>16950</v>
       </c>
       <c r="B231" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="232">
@@ -2290,7 +2290,7 @@
         <v>17000</v>
       </c>
       <c r="B232" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="233">
@@ -2298,7 +2298,7 @@
         <v>17000</v>
       </c>
       <c r="B233" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="234">
@@ -2306,7 +2306,7 @@
         <v>17000</v>
       </c>
       <c r="B234" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="235">
@@ -2314,7 +2314,7 @@
         <v>17000</v>
       </c>
       <c r="B235" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="236">
@@ -2322,7 +2322,7 @@
         <v>17000</v>
       </c>
       <c r="B236" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="237">
@@ -2330,7 +2330,7 @@
         <v>17000</v>
       </c>
       <c r="B237" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="238">
@@ -2338,7 +2338,7 @@
         <v>17000</v>
       </c>
       <c r="B238" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="239">
@@ -2346,7 +2346,7 @@
         <v>17000</v>
       </c>
       <c r="B239" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="240">
@@ -2354,7 +2354,7 @@
         <v>17000</v>
       </c>
       <c r="B240" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="241">
@@ -2362,7 +2362,7 @@
         <v>17000</v>
       </c>
       <c r="B241" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="242">
@@ -2370,7 +2370,7 @@
         <v>17000</v>
       </c>
       <c r="B242" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="243">
@@ -2378,7 +2378,7 @@
         <v>17000</v>
       </c>
       <c r="B243" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="244">
@@ -2386,7 +2386,7 @@
         <v>17000</v>
       </c>
       <c r="B244" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="245">
@@ -2394,7 +2394,7 @@
         <v>17000</v>
       </c>
       <c r="B245" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="246">
@@ -2402,7 +2402,7 @@
         <v>17000</v>
       </c>
       <c r="B246" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="247">
@@ -2410,7 +2410,7 @@
         <v>17000</v>
       </c>
       <c r="B247" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="248">
@@ -2418,7 +2418,7 @@
         <v>17000</v>
       </c>
       <c r="B248" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="249">
@@ -2426,7 +2426,7 @@
         <v>17000</v>
       </c>
       <c r="B249" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="250">
@@ -2434,7 +2434,7 @@
         <v>17000</v>
       </c>
       <c r="B250" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="251">
@@ -2442,7 +2442,7 @@
         <v>17000</v>
       </c>
       <c r="B251" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="252">
@@ -2450,7 +2450,7 @@
         <v>17000</v>
       </c>
       <c r="B252" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="253">
@@ -2458,7 +2458,7 @@
         <v>17000</v>
       </c>
       <c r="B253" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="254">
@@ -2466,7 +2466,7 @@
         <v>17000</v>
       </c>
       <c r="B254" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="255">
@@ -2474,7 +2474,7 @@
         <v>17000</v>
       </c>
       <c r="B255" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="256">
@@ -2482,7 +2482,7 @@
         <v>17000</v>
       </c>
       <c r="B256" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="257">
@@ -2490,7 +2490,7 @@
         <v>17000</v>
       </c>
       <c r="B257" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="258">
@@ -2498,7 +2498,7 @@
         <v>17000</v>
       </c>
       <c r="B258" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="259">
@@ -2506,7 +2506,7 @@
         <v>17000</v>
       </c>
       <c r="B259" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="260">
@@ -2514,7 +2514,7 @@
         <v>17000</v>
       </c>
       <c r="B260" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="261">
@@ -2522,7 +2522,7 @@
         <v>17000</v>
       </c>
       <c r="B261" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="262">
@@ -2530,7 +2530,7 @@
         <v>17000</v>
       </c>
       <c r="B262" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="263">
@@ -2538,7 +2538,7 @@
         <v>17000</v>
       </c>
       <c r="B263" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="264">
@@ -2546,7 +2546,7 @@
         <v>17250</v>
       </c>
       <c r="B264" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="265">
@@ -2554,7 +2554,7 @@
         <v>17250</v>
       </c>
       <c r="B265" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="266">
@@ -2562,7 +2562,7 @@
         <v>17500</v>
       </c>
       <c r="B266" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="267">
@@ -2570,7 +2570,7 @@
         <v>17500</v>
       </c>
       <c r="B267" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="268">
@@ -2578,7 +2578,7 @@
         <v>17500</v>
       </c>
       <c r="B268" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="269">
@@ -2586,7 +2586,7 @@
         <v>17500</v>
       </c>
       <c r="B269" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="270">
@@ -2594,7 +2594,7 @@
         <v>17500</v>
       </c>
       <c r="B270" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="271">
@@ -2602,7 +2602,7 @@
         <v>17500</v>
       </c>
       <c r="B271" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="272">
@@ -2610,7 +2610,7 @@
         <v>17555</v>
       </c>
       <c r="B272" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="273">
@@ -2618,7 +2618,7 @@
         <v>18000</v>
       </c>
       <c r="B273" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="274">
@@ -2626,7 +2626,7 @@
         <v>18000</v>
       </c>
       <c r="B274" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="275">
@@ -2634,7 +2634,7 @@
         <v>18000</v>
       </c>
       <c r="B275" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="276">
@@ -2642,7 +2642,7 @@
         <v>18000</v>
       </c>
       <c r="B276" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="277">
@@ -2650,7 +2650,7 @@
         <v>18000</v>
       </c>
       <c r="B277" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="278">
@@ -2658,7 +2658,7 @@
         <v>18000</v>
       </c>
       <c r="B278" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="279">
@@ -2666,7 +2666,7 @@
         <v>18000</v>
       </c>
       <c r="B279" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="280">
@@ -2674,7 +2674,7 @@
         <v>18000</v>
       </c>
       <c r="B280" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="281">
@@ -2682,7 +2682,7 @@
         <v>18000</v>
       </c>
       <c r="B281" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="282">
@@ -2690,7 +2690,7 @@
         <v>18000</v>
       </c>
       <c r="B282" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="283">
@@ -2698,7 +2698,7 @@
         <v>18000</v>
       </c>
       <c r="B283" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="284">
@@ -2706,7 +2706,7 @@
         <v>18000</v>
       </c>
       <c r="B284" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="285">
@@ -2714,7 +2714,7 @@
         <v>18000</v>
       </c>
       <c r="B285" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="286">
@@ -2722,7 +2722,7 @@
         <v>18000</v>
       </c>
       <c r="B286" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="287">
@@ -2730,7 +2730,7 @@
         <v>18000</v>
       </c>
       <c r="B287" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="288">
@@ -2738,7 +2738,7 @@
         <v>18000</v>
       </c>
       <c r="B288" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="289">
@@ -2746,7 +2746,7 @@
         <v>18000</v>
       </c>
       <c r="B289" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="290">
@@ -2754,7 +2754,7 @@
         <v>18000</v>
       </c>
       <c r="B290" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="291">
@@ -2762,7 +2762,7 @@
         <v>18000</v>
       </c>
       <c r="B291" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="292">
@@ -2770,7 +2770,7 @@
         <v>18000</v>
       </c>
       <c r="B292" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="293">
@@ -2778,7 +2778,7 @@
         <v>18000</v>
       </c>
       <c r="B293" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="294">
@@ -2786,7 +2786,7 @@
         <v>18000</v>
       </c>
       <c r="B294" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="295">
@@ -2794,7 +2794,7 @@
         <v>18000</v>
       </c>
       <c r="B295" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="296">
@@ -2802,7 +2802,7 @@
         <v>18000</v>
       </c>
       <c r="B296" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="297">
@@ -2810,7 +2810,7 @@
         <v>18000</v>
       </c>
       <c r="B297" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="298">
@@ -2818,7 +2818,7 @@
         <v>18000</v>
       </c>
       <c r="B298" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="299">
@@ -2826,7 +2826,7 @@
         <v>18000</v>
       </c>
       <c r="B299" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="300">
@@ -2834,7 +2834,7 @@
         <v>18000</v>
       </c>
       <c r="B300" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="301">
@@ -2842,7 +2842,7 @@
         <v>18000</v>
       </c>
       <c r="B301" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="302">
@@ -2850,7 +2850,7 @@
         <v>18000</v>
       </c>
       <c r="B302" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="303">
@@ -2858,7 +2858,7 @@
         <v>18000</v>
       </c>
       <c r="B303" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="304">
@@ -2866,7 +2866,7 @@
         <v>18000</v>
       </c>
       <c r="B304" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="305">
@@ -2874,7 +2874,7 @@
         <v>18000</v>
       </c>
       <c r="B305" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="306">
@@ -2882,7 +2882,7 @@
         <v>18000</v>
       </c>
       <c r="B306" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="307">
@@ -2890,7 +2890,7 @@
         <v>18000</v>
       </c>
       <c r="B307" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="308">
@@ -2898,7 +2898,7 @@
         <v>18000</v>
       </c>
       <c r="B308" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="309">
@@ -2906,7 +2906,7 @@
         <v>18000</v>
       </c>
       <c r="B309" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="310">
@@ -2914,7 +2914,7 @@
         <v>18000</v>
       </c>
       <c r="B310" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="311">
@@ -2922,7 +2922,7 @@
         <v>18000</v>
       </c>
       <c r="B311" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="312">
@@ -2930,7 +2930,7 @@
         <v>18000</v>
       </c>
       <c r="B312" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="313">
@@ -2938,7 +2938,7 @@
         <v>18000</v>
       </c>
       <c r="B313" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="314">
@@ -2946,7 +2946,7 @@
         <v>18000</v>
       </c>
       <c r="B314" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="315">
@@ -2954,7 +2954,7 @@
         <v>18250</v>
       </c>
       <c r="B315" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="316">
@@ -2962,7 +2962,7 @@
         <v>18250</v>
       </c>
       <c r="B316" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="317">
@@ -2970,7 +2970,7 @@
         <v>18500</v>
       </c>
       <c r="B317" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="318">
@@ -2978,7 +2978,7 @@
         <v>18500</v>
       </c>
       <c r="B318" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="319">
@@ -2986,7 +2986,7 @@
         <v>18500</v>
       </c>
       <c r="B319" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="320">
@@ -2994,7 +2994,7 @@
         <v>18500</v>
       </c>
       <c r="B320" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="321">
@@ -3002,7 +3002,7 @@
         <v>18500</v>
       </c>
       <c r="B321" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="322">
@@ -3010,7 +3010,7 @@
         <v>18500</v>
       </c>
       <c r="B322" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="323">
@@ -3018,7 +3018,7 @@
         <v>18500</v>
       </c>
       <c r="B323" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="324">
@@ -3026,7 +3026,7 @@
         <v>18500</v>
       </c>
       <c r="B324" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="325">
@@ -3034,7 +3034,7 @@
         <v>18500</v>
       </c>
       <c r="B325" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="326">
@@ -4146,7 +4146,7 @@
         <v>23500</v>
       </c>
       <c r="B464" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="465">
@@ -4154,7 +4154,7 @@
         <v>24000</v>
       </c>
       <c r="B465" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="466">
@@ -4162,7 +4162,7 @@
         <v>24000</v>
       </c>
       <c r="B466" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="467">
@@ -4170,7 +4170,7 @@
         <v>24000</v>
       </c>
       <c r="B467" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="468">
@@ -4178,7 +4178,7 @@
         <v>24000</v>
       </c>
       <c r="B468" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="469">
@@ -4186,7 +4186,7 @@
         <v>24000</v>
       </c>
       <c r="B469" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="470">
@@ -4194,7 +4194,7 @@
         <v>24000</v>
       </c>
       <c r="B470" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="471">
@@ -4202,7 +4202,7 @@
         <v>24000</v>
       </c>
       <c r="B471" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="472">
@@ -4210,7 +4210,7 @@
         <v>24000</v>
       </c>
       <c r="B472" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="473">
@@ -4218,7 +4218,7 @@
         <v>24900</v>
       </c>
       <c r="B473" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="474">
@@ -4226,7 +4226,7 @@
         <v>24950</v>
       </c>
       <c r="B474" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="475">
@@ -4234,7 +4234,7 @@
         <v>25000</v>
       </c>
       <c r="B475" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="476">
@@ -4242,7 +4242,7 @@
         <v>25000</v>
       </c>
       <c r="B476" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="477">
@@ -4250,7 +4250,7 @@
         <v>25000</v>
       </c>
       <c r="B477" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="478">
@@ -4258,7 +4258,7 @@
         <v>25000</v>
       </c>
       <c r="B478" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="479">
@@ -4266,7 +4266,7 @@
         <v>25000</v>
       </c>
       <c r="B479" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="480">
@@ -4274,7 +4274,7 @@
         <v>25000</v>
       </c>
       <c r="B480" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="481">
@@ -4282,7 +4282,7 @@
         <v>25000</v>
       </c>
       <c r="B481" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="482">
@@ -4290,7 +4290,7 @@
         <v>25000</v>
       </c>
       <c r="B482" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="483">
@@ -4298,7 +4298,7 @@
         <v>25000</v>
       </c>
       <c r="B483" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="484">
@@ -4306,7 +4306,7 @@
         <v>25000</v>
       </c>
       <c r="B484" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="485">
@@ -4314,7 +4314,7 @@
         <v>25000</v>
       </c>
       <c r="B485" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="486">
@@ -4322,7 +4322,7 @@
         <v>25000</v>
       </c>
       <c r="B486" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="487">
@@ -4330,7 +4330,7 @@
         <v>25000</v>
       </c>
       <c r="B487" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="488">
@@ -4338,7 +4338,7 @@
         <v>25000</v>
       </c>
       <c r="B488" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="489">
@@ -4346,7 +4346,7 @@
         <v>25000</v>
       </c>
       <c r="B489" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="490">
@@ -4354,7 +4354,7 @@
         <v>25000</v>
       </c>
       <c r="B490" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="491">
@@ -4362,7 +4362,7 @@
         <v>25000</v>
       </c>
       <c r="B491" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="492">
@@ -4370,7 +4370,7 @@
         <v>25000</v>
       </c>
       <c r="B492" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="493">
@@ -4378,7 +4378,7 @@
         <v>25000</v>
       </c>
       <c r="B493" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="494">
@@ -4386,7 +4386,7 @@
         <v>25000</v>
       </c>
       <c r="B494" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="495">
@@ -4394,7 +4394,7 @@
         <v>25000</v>
       </c>
       <c r="B495" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="496">
@@ -4402,7 +4402,7 @@
         <v>25000</v>
       </c>
       <c r="B496" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="497">
@@ -4410,7 +4410,7 @@
         <v>25000</v>
       </c>
       <c r="B497" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="498">
@@ -4418,7 +4418,7 @@
         <v>25000</v>
       </c>
       <c r="B498" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="499">
@@ -4426,7 +4426,7 @@
         <v>25000</v>
       </c>
       <c r="B499" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="500">
@@ -4434,7 +4434,7 @@
         <v>25000</v>
       </c>
       <c r="B500" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="501">
@@ -4442,7 +4442,7 @@
         <v>25000</v>
       </c>
       <c r="B501" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="502">
@@ -4450,7 +4450,7 @@
         <v>25000</v>
       </c>
       <c r="B502" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="503">
@@ -4458,7 +4458,7 @@
         <v>25000</v>
       </c>
       <c r="B503" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="504">
@@ -4466,7 +4466,7 @@
         <v>25000</v>
       </c>
       <c r="B504" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="505">
@@ -4474,7 +4474,7 @@
         <v>25000</v>
       </c>
       <c r="B505" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="506">
@@ -4482,7 +4482,7 @@
         <v>25000</v>
       </c>
       <c r="B506" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="507">
@@ -4490,7 +4490,7 @@
         <v>25000</v>
       </c>
       <c r="B507" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="508">
@@ -4498,7 +4498,7 @@
         <v>25500</v>
       </c>
       <c r="B508" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="509">
@@ -4506,7 +4506,7 @@
         <v>25500</v>
       </c>
       <c r="B509" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="510">
@@ -4514,7 +4514,7 @@
         <v>26000</v>
       </c>
       <c r="B510" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="511">
@@ -4522,7 +4522,7 @@
         <v>26000</v>
       </c>
       <c r="B511" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="512">
@@ -4530,7 +4530,7 @@
         <v>26000</v>
       </c>
       <c r="B512" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="513">
@@ -4538,7 +4538,7 @@
         <v>26000</v>
       </c>
       <c r="B513" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="514">
@@ -4546,7 +4546,7 @@
         <v>26000</v>
       </c>
       <c r="B514" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="515">
@@ -4554,7 +4554,7 @@
         <v>26000</v>
       </c>
       <c r="B515" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="516">
@@ -4562,7 +4562,7 @@
         <v>26000</v>
       </c>
       <c r="B516" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="517">
@@ -4570,7 +4570,7 @@
         <v>26000</v>
       </c>
       <c r="B517" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="518">
@@ -4578,7 +4578,7 @@
         <v>26000</v>
       </c>
       <c r="B518" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="519">

</xml_diff>